<commit_message>
21.06.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/June/All Details/20.06.2020/MC Bank Statement June 2020.xlsx
+++ b/2020/June/All Details/20.06.2020/MC Bank Statement June 2020.xlsx
@@ -1576,7 +1576,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1588,7 +1588,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1611,14 +1611,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3105,7 +3105,7 @@
   <dimension ref="A1:AL222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21.75" customHeight="1"/>
@@ -3331,7 +3331,7 @@
         <v>28</v>
       </c>
       <c r="E6" s="109">
-        <v>672285</v>
+        <v>611785</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="66"/>
@@ -3377,7 +3377,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="110">
-        <v>1555978</v>
+        <v>1616478</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="66"/>

</xml_diff>